<commit_message>
finish unit test, and add sumNum,sumMinute param judge, and add update answer siduation.
</commit_message>
<xml_diff>
--- a/单元测试用例.xlsx
+++ b/单元测试用例.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>页面</t>
   </si>
   <si>
-    <t>功能</t>
+    <t>模块</t>
   </si>
   <si>
     <t>用例类型</t>
@@ -45,15 +45,51 @@
     <t>登录</t>
   </si>
   <si>
+    <t>账号与密码</t>
+  </si>
+  <si>
+    <t>正常</t>
+  </si>
+  <si>
+    <t>账号为空，密码为空</t>
+  </si>
+  <si>
+    <t>提示“请输入您的账号”</t>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>账号为空，密码不为空</t>
+  </si>
+  <si>
+    <t>账号不为空，密码为空</t>
+  </si>
+  <si>
+    <t>提示“请输入您的密码”</t>
+  </si>
+  <si>
+    <t>账号存在，密码错误</t>
+  </si>
+  <si>
+    <t>提示“您的账号或密码错误”</t>
+  </si>
+  <si>
+    <t>账号不存在</t>
+  </si>
+  <si>
+    <t>账号存在，密码正确</t>
+  </si>
+  <si>
+    <t>登录成功，隐藏登录窗口，显示考试窗口</t>
+  </si>
+  <si>
     <t>考试</t>
   </si>
   <si>
     <t>剩余答题时间</t>
   </si>
   <si>
-    <t>正常</t>
-  </si>
-  <si>
     <t>小时递减，递减后不为0</t>
   </si>
   <si>
@@ -63,9 +99,6 @@
     <t>01:59:59</t>
   </si>
   <si>
-    <t>是</t>
-  </si>
-  <si>
     <t>小时递减，递减后为0</t>
   </si>
   <si>
@@ -162,6 +195,18 @@
     <t>100:00:00</t>
   </si>
   <si>
+    <t>异常</t>
+  </si>
+  <si>
+    <t>页面传入答题时间为负数</t>
+  </si>
+  <si>
+    <t>-60</t>
+  </si>
+  <si>
+    <t>进行错误提示</t>
+  </si>
+  <si>
     <t>答案选项按钮</t>
   </si>
   <si>
@@ -201,6 +246,18 @@
     <t>当前题所有答案选项都不高亮，上一题答案选项高亮</t>
   </si>
   <si>
+    <t>当前题更改答案</t>
+  </si>
+  <si>
+    <t>原答案选项不高亮，新答案选项高亮</t>
+  </si>
+  <si>
+    <t>当前题有过更改答案，从其余题切换查看当前题</t>
+  </si>
+  <si>
+    <t>当前题最后选择答案正确高亮</t>
+  </si>
+  <si>
     <t>题号按钮</t>
   </si>
   <si>
@@ -219,16 +276,13 @@
     <t>按钮变成灰色</t>
   </si>
   <si>
-    <t>异常</t>
-  </si>
-  <si>
     <t>页面传入题号数量大于32</t>
   </si>
   <si>
-    <t>进行错误提示</t>
-  </si>
-  <si>
     <t>页面传入题号数量大于题库数量</t>
+  </si>
+  <si>
+    <t>页面传入题号数量为负数</t>
   </si>
   <si>
     <t>题目区域</t>
@@ -269,8 +323,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -300,6 +354,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -329,13 +390,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -428,20 +482,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -449,6 +489,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -459,31 +513,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,163 +697,65 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -755,152 +861,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,17 +1019,47 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1273,10 +1409,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1310,404 +1446,697 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="4:7">
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7">
-      <c r="D5" s="2" t="s">
+      <c r="G5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="1" spans="4:7">
-      <c r="D6" s="2" t="s">
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7">
-      <c r="D7" s="2" t="s">
+      <c r="E8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7">
-      <c r="D8" s="2" t="s">
+      <c r="E9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7">
-      <c r="D9" s="2" t="s">
+      <c r="E10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" spans="4:7">
-      <c r="D10" s="2" t="s">
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" s="2" customFormat="1" spans="1:8">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="1" spans="4:7">
-      <c r="D11" s="2" t="s">
+      <c r="G11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7">
-      <c r="D12" s="2" t="s">
+      <c r="G12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7">
-      <c r="D13" s="2" t="s">
+      <c r="G13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" s="2" customFormat="1" spans="1:8">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7">
-      <c r="D14" s="2" t="s">
+      <c r="E15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:8">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="2" t="s">
+      <c r="E16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="F16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="4:7">
-      <c r="D16" s="2" t="s">
+      <c r="E17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7">
-      <c r="D17" s="2" t="s">
+      <c r="G17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="7" t="s">
+      <c r="E18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7">
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" s="2" customFormat="1" spans="4:7">
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7">
-      <c r="D20" s="2" t="s">
+      <c r="G19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="2" t="s">
+      <c r="E20" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="F20" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7">
-      <c r="D22" s="2" t="s">
+      <c r="G20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="10"/>
+      <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="C21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7">
-      <c r="D23" s="2" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7">
-      <c r="C24" s="2" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7">
-      <c r="D25" s="2" t="s">
+      <c r="G23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="2" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="G24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" s="2" customFormat="1" spans="1:8">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="4:7">
-      <c r="D27" s="2" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7">
-      <c r="D28" s="2" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="2" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="G27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7">
-      <c r="D30" s="2" t="s">
+      <c r="G28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="10"/>
+      <c r="B29" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="C29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="G29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="10"/>
+      <c r="B35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="10"/>
+      <c r="B38" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A39"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B20"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C8:C19"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C38:C39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>